<commit_message>
Initial commit: working backend and frontend
</commit_message>
<xml_diff>
--- a/data/CGL_MAINS_2025/responses.xlsx
+++ b/data/CGL_MAINS_2025/responses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,132 +449,32 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Total Marks</t>
+          <t>Final Marks</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Subject 1</t>
+          <t>Mathamatics</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Subject 2</t>
+          <t>Reasoning</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Subject 3</t>
+          <t>English</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Subject 4</t>
+          <t>GK</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Subject 5</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>S1_Attempt</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>S1_R</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>S1_W</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>S1_NA</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>S2_Attempt</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>S2_R</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>S2_W</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>S2_NA</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>S3_Attempt</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>S3_R</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>S3_W</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>S3_NA</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>S4_Attempt</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>S4_R</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>S4_W</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>S4_NA</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>S5_Attempt</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>S5_R</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>S5_W</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>S5_NA</t>
+          <t>Computer</t>
         </is>
       </c>
     </row>
@@ -605,7 +505,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="G2" t="n">
         <v>75</v>
@@ -621,66 +521,6 @@
       </c>
       <c r="K2" t="n">
         <v>26</v>
-      </c>
-      <c r="L2" t="n">
-        <v>29</v>
-      </c>
-      <c r="M2" t="n">
-        <v>26</v>
-      </c>
-      <c r="N2" t="n">
-        <v>3</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>30</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>45</v>
-      </c>
-      <c r="U2" t="n">
-        <v>42</v>
-      </c>
-      <c r="V2" t="n">
-        <v>3</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>11</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove manual name/roll input and auto-extract from response sheet
</commit_message>
<xml_diff>
--- a/data/CGL_MAINS_2025/responses.xlsx
+++ b/data/CGL_MAINS_2025/responses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +523,162 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Holesh</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OBC</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>298</v>
+      </c>
+      <c r="G3" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Holesh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OBC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>298</v>
+      </c>
+      <c r="G4" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Holesh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1232141</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>341</v>
+      </c>
+      <c r="G5" t="n">
+        <v>75</v>
+      </c>
+      <c r="H5" t="n">
+        <v>90</v>
+      </c>
+      <c r="I5" t="n">
+        <v>123</v>
+      </c>
+      <c r="J5" t="n">
+        <v>53</v>
+      </c>
+      <c r="K5" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HOLESH SHARMA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3010018033</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>UR</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Arunachal Pradesh</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>341</v>
+      </c>
+      <c r="G6" t="n">
+        <v>75</v>
+      </c>
+      <c r="H6" t="n">
+        <v>90</v>
+      </c>
+      <c r="I6" t="n">
+        <v>123</v>
+      </c>
+      <c r="J6" t="n">
+        <v>53</v>
+      </c>
+      <c r="K6" t="n">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prepare backend for Render deployment
</commit_message>
<xml_diff>
--- a/data/CGL_MAINS_2025/responses.xlsx
+++ b/data/CGL_MAINS_2025/responses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,229 +454,128 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Mathamatics</t>
+          <t>Math_Attempt</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Reasoning</t>
+          <t>Math_R</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Math_W</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>Math_NA</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Computer</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Holesh Sharma</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>UR</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>341</v>
-      </c>
-      <c r="G2" t="n">
-        <v>75</v>
-      </c>
-      <c r="H2" t="n">
-        <v>90</v>
-      </c>
-      <c r="I2" t="n">
-        <v>123</v>
-      </c>
-      <c r="J2" t="n">
-        <v>53</v>
-      </c>
-      <c r="K2" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Holesh</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>12312</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>OBC</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Chhattisgarh</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>298</v>
-      </c>
-      <c r="G3" t="n">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Holesh</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12312</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>OBC</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Chhattisgarh</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>298</v>
-      </c>
-      <c r="G4" t="n">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Holesh</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1232141</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>341</v>
-      </c>
-      <c r="G5" t="n">
-        <v>75</v>
-      </c>
-      <c r="H5" t="n">
-        <v>90</v>
-      </c>
-      <c r="I5" t="n">
-        <v>123</v>
-      </c>
-      <c r="J5" t="n">
-        <v>53</v>
-      </c>
-      <c r="K5" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>HOLESH SHARMA</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3010018033</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>UR</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Arunachal Pradesh</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>341</v>
-      </c>
-      <c r="G6" t="n">
-        <v>75</v>
-      </c>
-      <c r="H6" t="n">
-        <v>90</v>
-      </c>
-      <c r="I6" t="n">
-        <v>123</v>
-      </c>
-      <c r="J6" t="n">
-        <v>53</v>
-      </c>
-      <c r="K6" t="n">
-        <v>26</v>
+          <t>Math_Marks</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Reasoning_Attempt</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Reasoning_R</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Reasoning_W</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Reasoning_NA</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Reasoning_Marks</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>English_Attempt</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>English_R</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>English_W</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>English_NA</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>English_Marks</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>GK_Attempt</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>GK_R</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>GK_W</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>GK_NA</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>GK_Marks</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Computer_Attempt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Computer_R</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Computer_W</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Computer_NA</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Computer_Marks</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>